<commit_message>
single column selection implemented
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/boats_certificates.xlsx
+++ b/app/src/main/res/raw/boats_certificates.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7cfb192ce2913f5/Documents/Koc/App Project/Fiverr/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadshaheer/Desktop/Workplace/kocFleet/app/src/main/res/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{D02EA2A3-DDC3-0D44-8A27-86B8F4E0196C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{752BCD05-2833-4BFA-92A2-09D898C87B9F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20720" windowHeight="13420"/>
   </bookViews>
   <sheets>
     <sheet name="Boats Condition" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -670,12 +672,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -694,28 +696,28 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -723,14 +725,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -738,7 +740,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -746,7 +748,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -754,7 +756,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -839,7 +841,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -849,16 +851,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -970,12 +981,6 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1006,10 +1011,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1329,142 +1340,341 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DG380"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="CY1" sqref="CY1:CY1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection sqref="A1:DG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="3" max="3" width="6.5625" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.9375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.1875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5625" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="17.3125" customWidth="1"/>
-    <col min="12" max="12" width="16.625" customWidth="1"/>
-    <col min="13" max="13" width="15.375" customWidth="1"/>
-    <col min="14" max="14" width="68.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="55.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="57.3125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="57.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="53.4375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="41.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.3125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.75" customWidth="1"/>
-    <col min="25" max="25" width="75.3125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.8125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="43.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.8125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.6640625" customWidth="1"/>
+    <col min="25" max="25" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="28" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="34.5625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.4375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21.0625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.9375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="19.8125" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="25.6875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="24.9375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.25" customWidth="1"/>
-    <col min="56" max="56" width="10.9375" customWidth="1"/>
-    <col min="57" max="57" width="11.4375" customWidth="1"/>
-    <col min="59" max="59" width="10.5" customWidth="1"/>
-    <col min="60" max="60" width="10.5625" customWidth="1"/>
-    <col min="61" max="61" width="35.6875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.8125" customWidth="1"/>
-    <col min="63" max="63" width="10.5625" customWidth="1"/>
-    <col min="64" max="64" width="39.6875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="30.75" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="42.4375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="39.875" customWidth="1"/>
-    <col min="74" max="74" width="37.875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="18.6875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="54.8125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="55.375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.1640625" customWidth="1"/>
+    <col min="56" max="56" width="11" customWidth="1"/>
+    <col min="57" max="57" width="11.5" customWidth="1"/>
+    <col min="59" max="60" width="10.5" customWidth="1"/>
+    <col min="61" max="61" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.83203125" customWidth="1"/>
+    <col min="63" max="63" width="10.5" customWidth="1"/>
+    <col min="64" max="64" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="39.83203125" customWidth="1"/>
+    <col min="74" max="74" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="26.5" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="28" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="39.9375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="26.9375" bestFit="1" customWidth="1"/>
-    <col min="85" max="86" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="40" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="17" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="25" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="65.8125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="51.75" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="12.1875" customWidth="1"/>
-    <col min="93" max="94" width="10.4375" customWidth="1"/>
-    <col min="95" max="95" width="50.9375" bestFit="1" customWidth="1"/>
-    <col min="96" max="97" width="10.4375" customWidth="1"/>
-    <col min="98" max="98" width="10.3125" customWidth="1"/>
-    <col min="99" max="99" width="9.75" customWidth="1"/>
-    <col min="100" max="100" width="40.375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="17.3125" customWidth="1"/>
-    <col min="102" max="102" width="17.75" customWidth="1"/>
-    <col min="103" max="103" width="86.375" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="59.375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="66.6875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="57.1875" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="17.9375" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="46.3125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="9.4375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="12.1640625" customWidth="1"/>
+    <col min="93" max="94" width="10.5" customWidth="1"/>
+    <col min="95" max="95" width="51" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="10.5" customWidth="1"/>
+    <col min="98" max="98" width="10.33203125" customWidth="1"/>
+    <col min="99" max="99" width="9.6640625" customWidth="1"/>
+    <col min="100" max="100" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="17.33203125" customWidth="1"/>
+    <col min="102" max="102" width="17.6640625" customWidth="1"/>
+    <col min="103" max="103" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="18" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:111" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:111" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:111" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-    </row>
-    <row r="3" spans="1:111" s="34" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+      <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="48"/>
+      <c r="AZ1" s="48"/>
+      <c r="BA1" s="48"/>
+      <c r="BB1" s="48"/>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="48"/>
+      <c r="BR1" s="48"/>
+      <c r="BS1" s="48"/>
+      <c r="BT1" s="48"/>
+      <c r="BU1" s="48"/>
+      <c r="BV1" s="48"/>
+      <c r="BW1" s="48"/>
+      <c r="BX1" s="48"/>
+      <c r="BY1" s="48"/>
+      <c r="BZ1" s="48"/>
+      <c r="CA1" s="48"/>
+      <c r="CB1" s="48"/>
+      <c r="CC1" s="48"/>
+      <c r="CD1" s="48"/>
+      <c r="CE1" s="48"/>
+      <c r="CF1" s="48"/>
+      <c r="CG1" s="48"/>
+      <c r="CH1" s="48"/>
+      <c r="CI1" s="48"/>
+      <c r="CJ1" s="48"/>
+      <c r="CK1" s="48"/>
+      <c r="CL1" s="48"/>
+      <c r="CM1" s="48"/>
+      <c r="CN1" s="48"/>
+      <c r="CO1" s="48"/>
+      <c r="CP1" s="48"/>
+      <c r="CQ1" s="48"/>
+      <c r="CR1" s="48"/>
+      <c r="CS1" s="48"/>
+      <c r="CT1" s="48"/>
+      <c r="CU1" s="48"/>
+      <c r="CV1" s="48"/>
+      <c r="CW1" s="48"/>
+      <c r="CX1" s="48"/>
+      <c r="CY1" s="48"/>
+      <c r="CZ1" s="48"/>
+      <c r="DA1" s="48"/>
+      <c r="DB1" s="48"/>
+      <c r="DC1" s="48"/>
+      <c r="DD1" s="48"/>
+      <c r="DE1" s="48"/>
+      <c r="DF1" s="48"/>
+      <c r="DG1" s="48"/>
+    </row>
+    <row r="2" spans="1:111" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="49"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="49"/>
+      <c r="AU2" s="49"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="49"/>
+      <c r="BB2" s="49"/>
+      <c r="BC2" s="49"/>
+      <c r="BD2" s="49"/>
+      <c r="BE2" s="49"/>
+      <c r="BF2" s="49"/>
+      <c r="BG2" s="49"/>
+      <c r="BH2" s="49"/>
+      <c r="BI2" s="49"/>
+      <c r="BJ2" s="49"/>
+      <c r="BK2" s="49"/>
+      <c r="BL2" s="49"/>
+      <c r="BM2" s="49"/>
+      <c r="BN2" s="49"/>
+      <c r="BO2" s="49"/>
+      <c r="BP2" s="49"/>
+      <c r="BQ2" s="49"/>
+      <c r="BR2" s="49"/>
+      <c r="BS2" s="49"/>
+      <c r="BT2" s="49"/>
+      <c r="BU2" s="49"/>
+      <c r="BV2" s="49"/>
+      <c r="BW2" s="49"/>
+      <c r="BX2" s="49"/>
+      <c r="BY2" s="49"/>
+      <c r="BZ2" s="49"/>
+      <c r="CA2" s="49"/>
+      <c r="CB2" s="49"/>
+      <c r="CC2" s="49"/>
+      <c r="CD2" s="49"/>
+      <c r="CE2" s="49"/>
+      <c r="CF2" s="49"/>
+      <c r="CG2" s="49"/>
+      <c r="CH2" s="49"/>
+      <c r="CI2" s="49"/>
+      <c r="CJ2" s="49"/>
+      <c r="CK2" s="49"/>
+      <c r="CL2" s="49"/>
+      <c r="CM2" s="49"/>
+      <c r="CN2" s="49"/>
+      <c r="CO2" s="49"/>
+      <c r="CP2" s="49"/>
+      <c r="CQ2" s="49"/>
+      <c r="CR2" s="49"/>
+      <c r="CS2" s="49"/>
+      <c r="CT2" s="49"/>
+      <c r="CU2" s="49"/>
+      <c r="CV2" s="49"/>
+      <c r="CW2" s="49"/>
+      <c r="CX2" s="49"/>
+      <c r="CY2" s="49"/>
+      <c r="CZ2" s="49"/>
+      <c r="DA2" s="49"/>
+      <c r="DB2" s="49"/>
+      <c r="DC2" s="49"/>
+      <c r="DD2" s="49"/>
+      <c r="DE2" s="49"/>
+      <c r="DF2" s="49"/>
+      <c r="DG2" s="49"/>
+    </row>
+    <row r="3" spans="1:111" s="34" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="35">
         <v>1</v>
       </c>
@@ -1790,10 +2000,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:111" s="27" customFormat="1" ht="135" x14ac:dyDescent="0.35">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+    <row r="4" spans="1:111" s="27" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="25" t="s">
         <v>103</v>
       </c>
@@ -2119,14 +2329,14 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="42" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="33">
@@ -2240,7 +2450,7 @@
       <c r="DF5" s="24"/>
       <c r="DG5" s="24"/>
     </row>
-    <row r="6" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
         <f>+A5+1</f>
         <v>2</v>
@@ -2248,7 +2458,7 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -2358,7 +2568,7 @@
       <c r="DF6" s="24"/>
       <c r="DG6" s="24"/>
     </row>
-    <row r="7" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <f t="shared" ref="A7:A68" si="0">+A6+1</f>
         <v>3</v>
@@ -2366,7 +2576,7 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -2476,7 +2686,7 @@
       <c r="DF7" s="24"/>
       <c r="DG7" s="24"/>
     </row>
-    <row r="8" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2484,7 +2694,7 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -2594,7 +2804,7 @@
       <c r="DF8" s="24"/>
       <c r="DG8" s="24"/>
     </row>
-    <row r="9" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2602,7 +2812,7 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="44"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -2712,7 +2922,7 @@
       <c r="DF9" s="24"/>
       <c r="DG9" s="24"/>
     </row>
-    <row r="10" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2720,7 +2930,7 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="16"/>
@@ -2832,7 +3042,7 @@
       <c r="DF10" s="24"/>
       <c r="DG10" s="24"/>
     </row>
-    <row r="11" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2840,7 +3050,7 @@
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -2950,7 +3160,7 @@
       <c r="DF11" s="24"/>
       <c r="DG11" s="24"/>
     </row>
-    <row r="12" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2958,7 +3168,7 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -3068,7 +3278,7 @@
       <c r="DF12" s="24"/>
       <c r="DG12" s="24"/>
     </row>
-    <row r="13" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3076,7 +3286,7 @@
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -3186,7 +3396,7 @@
       <c r="DF13" s="24"/>
       <c r="DG13" s="24"/>
     </row>
-    <row r="14" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3194,7 +3404,7 @@
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="43"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -3304,7 +3514,7 @@
       <c r="DF14" s="24"/>
       <c r="DG14" s="24"/>
     </row>
-    <row r="15" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3312,7 +3522,7 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -3422,7 +3632,7 @@
       <c r="DF15" s="24"/>
       <c r="DG15" s="24"/>
     </row>
-    <row r="16" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3430,7 +3640,7 @@
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -3540,7 +3750,7 @@
       <c r="DF16" s="24"/>
       <c r="DG16" s="24"/>
     </row>
-    <row r="17" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3548,7 +3758,7 @@
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="43"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -3658,7 +3868,7 @@
       <c r="DF17" s="24"/>
       <c r="DG17" s="24"/>
     </row>
-    <row r="18" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3666,7 +3876,7 @@
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -3776,7 +3986,7 @@
       <c r="DF18" s="24"/>
       <c r="DG18" s="24"/>
     </row>
-    <row r="19" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3784,7 +3994,7 @@
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="42" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="16"/>
@@ -3896,7 +4106,7 @@
       <c r="DF19" s="24"/>
       <c r="DG19" s="24"/>
     </row>
-    <row r="20" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3904,7 +4114,7 @@
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -4014,7 +4224,7 @@
       <c r="DF20" s="24"/>
       <c r="DG20" s="24"/>
     </row>
-    <row r="21" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4022,7 +4232,7 @@
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -4132,7 +4342,7 @@
       <c r="DF21" s="24"/>
       <c r="DG21" s="24"/>
     </row>
-    <row r="22" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4140,7 +4350,7 @@
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -4250,7 +4460,7 @@
       <c r="DF22" s="24"/>
       <c r="DG22" s="24"/>
     </row>
-    <row r="23" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4258,7 +4468,7 @@
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -4368,7 +4578,7 @@
       <c r="DF23" s="24"/>
       <c r="DG23" s="24"/>
     </row>
-    <row r="24" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4376,7 +4586,7 @@
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="16"/>
@@ -4488,7 +4698,7 @@
       <c r="DF24" s="24"/>
       <c r="DG24" s="24"/>
     </row>
-    <row r="25" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4496,7 +4706,7 @@
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="45"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -4606,7 +4816,7 @@
       <c r="DF25" s="24"/>
       <c r="DG25" s="24"/>
     </row>
-    <row r="26" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4614,7 +4824,7 @@
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="45"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -4724,7 +4934,7 @@
       <c r="DF26" s="24"/>
       <c r="DG26" s="24"/>
     </row>
-    <row r="27" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4732,7 +4942,7 @@
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="45"/>
+      <c r="C27" s="43"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -4842,7 +5052,7 @@
       <c r="DF27" s="24"/>
       <c r="DG27" s="24"/>
     </row>
-    <row r="28" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4850,7 +5060,7 @@
       <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="45"/>
+      <c r="C28" s="43"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -4960,7 +5170,7 @@
       <c r="DF28" s="24"/>
       <c r="DG28" s="24"/>
     </row>
-    <row r="29" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4968,7 +5178,7 @@
       <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="45"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -5078,7 +5288,7 @@
       <c r="DF29" s="24"/>
       <c r="DG29" s="24"/>
     </row>
-    <row r="30" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5086,7 +5296,7 @@
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="16"/>
@@ -5198,7 +5408,7 @@
       <c r="DF30" s="24"/>
       <c r="DG30" s="24"/>
     </row>
-    <row r="31" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5206,7 +5416,7 @@
       <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="46"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
@@ -5316,7 +5526,7 @@
       <c r="DF31" s="24"/>
       <c r="DG31" s="24"/>
     </row>
-    <row r="32" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5324,7 +5534,7 @@
       <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="46"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
@@ -5434,7 +5644,7 @@
       <c r="DF32" s="24"/>
       <c r="DG32" s="24"/>
     </row>
-    <row r="33" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5442,7 +5652,7 @@
       <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="46"/>
+      <c r="C33" s="44"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
@@ -5552,7 +5762,7 @@
       <c r="DF33" s="24"/>
       <c r="DG33" s="24"/>
     </row>
-    <row r="34" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5560,7 +5770,7 @@
       <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="46"/>
+      <c r="C34" s="44"/>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -5670,7 +5880,7 @@
       <c r="DF34" s="24"/>
       <c r="DG34" s="24"/>
     </row>
-    <row r="35" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="30">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5678,7 +5888,7 @@
       <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="46"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -5788,7 +5998,7 @@
       <c r="DF35" s="24"/>
       <c r="DG35" s="24"/>
     </row>
-    <row r="36" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="30">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -5796,7 +6006,7 @@
       <c r="B36" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="46"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
@@ -5906,7 +6116,7 @@
       <c r="DF36" s="24"/>
       <c r="DG36" s="24"/>
     </row>
-    <row r="37" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="30">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5914,7 +6124,7 @@
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="46"/>
+      <c r="C37" s="44"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -6024,7 +6234,7 @@
       <c r="DF37" s="24"/>
       <c r="DG37" s="24"/>
     </row>
-    <row r="38" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -6032,7 +6242,7 @@
       <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="46"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
@@ -6142,7 +6352,7 @@
       <c r="DF38" s="24"/>
       <c r="DG38" s="24"/>
     </row>
-    <row r="39" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -6150,7 +6360,7 @@
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="46"/>
+      <c r="C39" s="44"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
@@ -6260,7 +6470,7 @@
       <c r="DF39" s="24"/>
       <c r="DG39" s="24"/>
     </row>
-    <row r="40" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="30">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -6268,7 +6478,7 @@
       <c r="B40" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="45" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="16"/>
@@ -6380,7 +6590,7 @@
       <c r="DF40" s="24"/>
       <c r="DG40" s="24"/>
     </row>
-    <row r="41" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -6388,7 +6598,7 @@
       <c r="B41" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="47"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -6498,7 +6708,7 @@
       <c r="DF41" s="24"/>
       <c r="DG41" s="24"/>
     </row>
-    <row r="42" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -6506,7 +6716,7 @@
       <c r="B42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="47"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
@@ -6616,7 +6826,7 @@
       <c r="DF42" s="24"/>
       <c r="DG42" s="24"/>
     </row>
-    <row r="43" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -6624,7 +6834,7 @@
       <c r="B43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="47"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
@@ -6734,7 +6944,7 @@
       <c r="DF43" s="24"/>
       <c r="DG43" s="24"/>
     </row>
-    <row r="44" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6742,7 +6952,7 @@
       <c r="B44" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="47"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -6852,7 +7062,7 @@
       <c r="DF44" s="24"/>
       <c r="DG44" s="24"/>
     </row>
-    <row r="45" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="30">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6860,7 +7070,7 @@
       <c r="B45" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="47"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
@@ -6970,7 +7180,7 @@
       <c r="DF45" s="24"/>
       <c r="DG45" s="24"/>
     </row>
-    <row r="46" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="30">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6978,7 +7188,7 @@
       <c r="B46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="47"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
@@ -7088,7 +7298,7 @@
       <c r="DF46" s="24"/>
       <c r="DG46" s="24"/>
     </row>
-    <row r="47" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -7096,7 +7306,7 @@
       <c r="B47" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="47"/>
+      <c r="C47" s="45"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
@@ -7206,7 +7416,7 @@
       <c r="DF47" s="24"/>
       <c r="DG47" s="24"/>
     </row>
-    <row r="48" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="30">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -7214,7 +7424,7 @@
       <c r="B48" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="48" t="s">
+      <c r="C48" s="46" t="s">
         <v>51</v>
       </c>
       <c r="D48" s="16"/>
@@ -7326,7 +7536,7 @@
       <c r="DF48" s="24"/>
       <c r="DG48" s="24"/>
     </row>
-    <row r="49" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="30">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -7334,7 +7544,7 @@
       <c r="B49" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="48"/>
+      <c r="C49" s="46"/>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
       <c r="F49" s="16"/>
@@ -7444,7 +7654,7 @@
       <c r="DF49" s="24"/>
       <c r="DG49" s="24"/>
     </row>
-    <row r="50" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -7452,7 +7662,7 @@
       <c r="B50" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="48"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
       <c r="F50" s="16"/>
@@ -7562,7 +7772,7 @@
       <c r="DF50" s="24"/>
       <c r="DG50" s="24"/>
     </row>
-    <row r="51" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="30">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -7570,7 +7780,7 @@
       <c r="B51" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="48"/>
+      <c r="C51" s="46"/>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
       <c r="F51" s="16"/>
@@ -7680,7 +7890,7 @@
       <c r="DF51" s="24"/>
       <c r="DG51" s="24"/>
     </row>
-    <row r="52" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="30">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -7688,7 +7898,7 @@
       <c r="B52" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="48"/>
+      <c r="C52" s="46"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
       <c r="F52" s="16"/>
@@ -7798,7 +8008,7 @@
       <c r="DF52" s="24"/>
       <c r="DG52" s="24"/>
     </row>
-    <row r="53" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="30">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -7806,7 +8016,7 @@
       <c r="B53" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="48"/>
+      <c r="C53" s="46"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="16"/>
@@ -7916,7 +8126,7 @@
       <c r="DF53" s="24"/>
       <c r="DG53" s="24"/>
     </row>
-    <row r="54" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -7924,7 +8134,7 @@
       <c r="B54" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="48"/>
+      <c r="C54" s="46"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
       <c r="F54" s="16"/>
@@ -8034,7 +8244,7 @@
       <c r="DF54" s="24"/>
       <c r="DG54" s="24"/>
     </row>
-    <row r="55" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="30">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -8042,7 +8252,7 @@
       <c r="B55" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="48"/>
+      <c r="C55" s="46"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16"/>
@@ -8152,7 +8362,7 @@
       <c r="DF55" s="24"/>
       <c r="DG55" s="24"/>
     </row>
-    <row r="56" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -8160,7 +8370,7 @@
       <c r="B56" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="48"/>
+      <c r="C56" s="46"/>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
       <c r="F56" s="16"/>
@@ -8270,7 +8480,7 @@
       <c r="DF56" s="24"/>
       <c r="DG56" s="24"/>
     </row>
-    <row r="57" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -8278,7 +8488,7 @@
       <c r="B57" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C57" s="38" t="s">
         <v>61</v>
       </c>
       <c r="D57" s="16"/>
@@ -8390,7 +8600,7 @@
       <c r="DF57" s="24"/>
       <c r="DG57" s="24"/>
     </row>
-    <row r="58" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -8398,7 +8608,7 @@
       <c r="B58" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="40"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
       <c r="F58" s="16"/>
@@ -8508,7 +8718,7 @@
       <c r="DF58" s="24"/>
       <c r="DG58" s="24"/>
     </row>
-    <row r="59" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -8516,7 +8726,7 @@
       <c r="B59" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="40"/>
+      <c r="C59" s="38"/>
       <c r="D59" s="19"/>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
@@ -8626,7 +8836,7 @@
       <c r="DF59" s="24"/>
       <c r="DG59" s="24"/>
     </row>
-    <row r="60" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -8634,7 +8844,7 @@
       <c r="B60" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="39" t="s">
         <v>65</v>
       </c>
       <c r="D60" s="16"/>
@@ -8746,7 +8956,7 @@
       <c r="DF60" s="24"/>
       <c r="DG60" s="24"/>
     </row>
-    <row r="61" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -8754,7 +8964,7 @@
       <c r="B61" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="41"/>
+      <c r="C61" s="39"/>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
       <c r="F61" s="16"/>
@@ -8864,7 +9074,7 @@
       <c r="DF61" s="24"/>
       <c r="DG61" s="24"/>
     </row>
-    <row r="62" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -8872,7 +9082,7 @@
       <c r="B62" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="41"/>
+      <c r="C62" s="39"/>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
@@ -8982,7 +9192,7 @@
       <c r="DF62" s="24"/>
       <c r="DG62" s="24"/>
     </row>
-    <row r="63" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="30">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -8990,7 +9200,7 @@
       <c r="B63" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="41"/>
+      <c r="C63" s="39"/>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
       <c r="F63" s="19"/>
@@ -9100,7 +9310,7 @@
       <c r="DF63" s="24"/>
       <c r="DG63" s="24"/>
     </row>
-    <row r="64" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -9108,7 +9318,7 @@
       <c r="B64" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="41"/>
+      <c r="C64" s="39"/>
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
       <c r="F64" s="19"/>
@@ -9218,7 +9428,7 @@
       <c r="DF64" s="24"/>
       <c r="DG64" s="24"/>
     </row>
-    <row r="65" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -9226,7 +9436,7 @@
       <c r="B65" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="41"/>
+      <c r="C65" s="39"/>
       <c r="D65" s="19"/>
       <c r="E65" s="19"/>
       <c r="F65" s="19"/>
@@ -9336,7 +9546,7 @@
       <c r="DF65" s="24"/>
       <c r="DG65" s="24"/>
     </row>
-    <row r="66" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -9344,7 +9554,7 @@
       <c r="B66" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C66" s="42" t="s">
+      <c r="C66" s="40" t="s">
         <v>72</v>
       </c>
       <c r="D66" s="16"/>
@@ -9456,7 +9666,7 @@
       <c r="DF66" s="24"/>
       <c r="DG66" s="24"/>
     </row>
-    <row r="67" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -9464,7 +9674,7 @@
       <c r="B67" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="42"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
@@ -9574,7 +9784,7 @@
       <c r="DF67" s="24"/>
       <c r="DG67" s="24"/>
     </row>
-    <row r="68" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:111" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -9582,7 +9792,7 @@
       <c r="B68" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="42"/>
+      <c r="C68" s="40"/>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
       <c r="F68" s="19"/>
@@ -9692,2184 +9902,2184 @@
       <c r="DF68" s="24"/>
       <c r="DG68" s="24"/>
     </row>
-    <row r="69" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
     </row>
-    <row r="70" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" s="15"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
       <c r="E71" s="15"/>
       <c r="F71" s="15"/>
       <c r="G71" s="15"/>
     </row>
-    <row r="72" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
       <c r="E72" s="15"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
     </row>
-    <row r="73" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
     </row>
-    <row r="74" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
     </row>
-    <row r="75" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
       <c r="E75" s="15"/>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
     </row>
-    <row r="76" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
       <c r="E76" s="15"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
     </row>
-    <row r="77" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
     </row>
-    <row r="78" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
     </row>
-    <row r="79" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
     </row>
-    <row r="80" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:111" x14ac:dyDescent="0.2">
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C84" s="15"/>
       <c r="D84" s="15"/>
       <c r="E84" s="15"/>
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C85" s="15"/>
       <c r="D85" s="15"/>
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
       <c r="G85" s="15"/>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C86" s="15"/>
       <c r="D86" s="15"/>
       <c r="E86" s="15"/>
       <c r="F86" s="15"/>
       <c r="G86" s="15"/>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C87" s="15"/>
       <c r="D87" s="15"/>
       <c r="E87" s="15"/>
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C88" s="15"/>
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C89" s="15"/>
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C90" s="15"/>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C92" s="15"/>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C94" s="15"/>
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C96" s="15"/>
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
     </row>
-    <row r="97" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C97" s="15"/>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
       <c r="F97" s="15"/>
       <c r="G97" s="15"/>
     </row>
-    <row r="98" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C98" s="15"/>
       <c r="D98" s="15"/>
       <c r="E98" s="15"/>
       <c r="F98" s="15"/>
       <c r="G98" s="15"/>
     </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C99" s="15"/>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
       <c r="F99" s="15"/>
       <c r="G99" s="15"/>
     </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
       <c r="E100" s="15"/>
       <c r="F100" s="15"/>
       <c r="G100" s="15"/>
     </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C101" s="15"/>
       <c r="D101" s="15"/>
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
     </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C102" s="15"/>
       <c r="D102" s="15"/>
       <c r="E102" s="15"/>
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
     </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C103" s="15"/>
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
       <c r="F103" s="15"/>
       <c r="G103" s="15"/>
     </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C104" s="15"/>
       <c r="D104" s="15"/>
       <c r="E104" s="15"/>
       <c r="F104" s="15"/>
       <c r="G104" s="15"/>
     </row>
-    <row r="105" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C105" s="15"/>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
       <c r="F105" s="15"/>
       <c r="G105" s="15"/>
     </row>
-    <row r="106" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C106" s="15"/>
       <c r="D106" s="15"/>
       <c r="E106" s="15"/>
       <c r="F106" s="15"/>
       <c r="G106" s="15"/>
     </row>
-    <row r="107" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C107" s="15"/>
       <c r="D107" s="15"/>
       <c r="E107" s="15"/>
       <c r="F107" s="15"/>
       <c r="G107" s="15"/>
     </row>
-    <row r="108" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C108" s="15"/>
       <c r="D108" s="15"/>
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
       <c r="G108" s="15"/>
     </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C109" s="15"/>
       <c r="D109" s="15"/>
       <c r="E109" s="15"/>
       <c r="F109" s="15"/>
       <c r="G109" s="15"/>
     </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C110" s="15"/>
       <c r="D110" s="15"/>
       <c r="E110" s="15"/>
       <c r="F110" s="15"/>
       <c r="G110" s="15"/>
     </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C111" s="15"/>
       <c r="D111" s="15"/>
       <c r="E111" s="15"/>
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
     </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C112" s="15"/>
       <c r="D112" s="15"/>
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C113" s="15"/>
       <c r="D113" s="15"/>
       <c r="E113" s="15"/>
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C114" s="15"/>
       <c r="D114" s="15"/>
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
       <c r="G114" s="15"/>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C115" s="15"/>
       <c r="D115" s="15"/>
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
     </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C116" s="15"/>
       <c r="D116" s="15"/>
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
       <c r="G116" s="15"/>
     </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C117" s="15"/>
       <c r="D117" s="15"/>
       <c r="E117" s="15"/>
       <c r="F117" s="15"/>
       <c r="G117" s="15"/>
     </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C118" s="15"/>
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
       <c r="F118" s="15"/>
       <c r="G118" s="15"/>
     </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C119" s="15"/>
       <c r="D119" s="15"/>
       <c r="E119" s="15"/>
       <c r="F119" s="15"/>
       <c r="G119" s="15"/>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C120" s="15"/>
       <c r="D120" s="15"/>
       <c r="E120" s="15"/>
       <c r="F120" s="15"/>
       <c r="G120" s="15"/>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C121" s="15"/>
       <c r="D121" s="15"/>
       <c r="E121" s="15"/>
       <c r="F121" s="15"/>
       <c r="G121" s="15"/>
     </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C122" s="15"/>
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="15"/>
       <c r="G122" s="15"/>
     </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C123" s="15"/>
       <c r="D123" s="15"/>
       <c r="E123" s="15"/>
       <c r="F123" s="15"/>
       <c r="G123" s="15"/>
     </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C124" s="15"/>
       <c r="D124" s="15"/>
       <c r="E124" s="15"/>
       <c r="F124" s="15"/>
       <c r="G124" s="15"/>
     </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
       <c r="E125" s="15"/>
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
     </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C126" s="15"/>
       <c r="D126" s="15"/>
       <c r="E126" s="15"/>
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
     </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
       <c r="E127" s="15"/>
       <c r="F127" s="15"/>
       <c r="G127" s="15"/>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C128" s="15"/>
       <c r="D128" s="15"/>
       <c r="E128" s="15"/>
       <c r="F128" s="15"/>
       <c r="G128" s="15"/>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C129" s="15"/>
       <c r="D129" s="15"/>
       <c r="E129" s="15"/>
       <c r="F129" s="15"/>
       <c r="G129" s="15"/>
     </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C130" s="15"/>
       <c r="D130" s="15"/>
       <c r="E130" s="15"/>
       <c r="F130" s="15"/>
       <c r="G130" s="15"/>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C131" s="15"/>
       <c r="D131" s="15"/>
       <c r="E131" s="15"/>
       <c r="F131" s="15"/>
       <c r="G131" s="15"/>
     </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C132" s="15"/>
       <c r="D132" s="15"/>
       <c r="E132" s="15"/>
       <c r="F132" s="15"/>
       <c r="G132" s="15"/>
     </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C133" s="15"/>
       <c r="D133" s="15"/>
       <c r="E133" s="15"/>
       <c r="F133" s="15"/>
       <c r="G133" s="15"/>
     </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C134" s="15"/>
       <c r="D134" s="15"/>
       <c r="E134" s="15"/>
       <c r="F134" s="15"/>
       <c r="G134" s="15"/>
     </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C135" s="15"/>
       <c r="D135" s="15"/>
       <c r="E135" s="15"/>
       <c r="F135" s="15"/>
       <c r="G135" s="15"/>
     </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C136" s="15"/>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
       <c r="F136" s="15"/>
       <c r="G136" s="15"/>
     </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C137" s="15"/>
       <c r="D137" s="15"/>
       <c r="E137" s="15"/>
       <c r="F137" s="15"/>
       <c r="G137" s="15"/>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C138" s="15"/>
       <c r="D138" s="15"/>
       <c r="E138" s="15"/>
       <c r="F138" s="15"/>
       <c r="G138" s="15"/>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C139" s="15"/>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
       <c r="F139" s="15"/>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C140" s="15"/>
       <c r="D140" s="15"/>
       <c r="E140" s="15"/>
       <c r="F140" s="15"/>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C141" s="15"/>
       <c r="D141" s="15"/>
       <c r="E141" s="15"/>
       <c r="F141" s="15"/>
       <c r="G141" s="15"/>
     </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C142" s="15"/>
       <c r="D142" s="15"/>
       <c r="E142" s="15"/>
       <c r="F142" s="15"/>
       <c r="G142" s="15"/>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C143" s="15"/>
       <c r="D143" s="15"/>
       <c r="E143" s="15"/>
       <c r="F143" s="15"/>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C144" s="15"/>
       <c r="D144" s="15"/>
       <c r="E144" s="15"/>
       <c r="F144" s="15"/>
       <c r="G144" s="15"/>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C145" s="15"/>
       <c r="D145" s="15"/>
       <c r="E145" s="15"/>
       <c r="F145" s="15"/>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C146" s="15"/>
       <c r="D146" s="15"/>
       <c r="E146" s="15"/>
       <c r="F146" s="15"/>
       <c r="G146" s="15"/>
     </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C147" s="15"/>
       <c r="D147" s="15"/>
       <c r="E147" s="15"/>
       <c r="F147" s="15"/>
       <c r="G147" s="15"/>
     </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C148" s="15"/>
       <c r="D148" s="15"/>
       <c r="E148" s="15"/>
       <c r="F148" s="15"/>
       <c r="G148" s="15"/>
     </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C149" s="15"/>
       <c r="D149" s="15"/>
       <c r="E149" s="15"/>
       <c r="F149" s="15"/>
       <c r="G149" s="15"/>
     </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C150" s="15"/>
       <c r="D150" s="15"/>
       <c r="E150" s="15"/>
       <c r="F150" s="15"/>
       <c r="G150" s="15"/>
     </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C151" s="15"/>
       <c r="D151" s="15"/>
       <c r="E151" s="15"/>
       <c r="F151" s="15"/>
       <c r="G151" s="15"/>
     </row>
-    <row r="152" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C152" s="15"/>
       <c r="D152" s="15"/>
       <c r="E152" s="15"/>
       <c r="F152" s="15"/>
       <c r="G152" s="15"/>
     </row>
-    <row r="153" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C153" s="15"/>
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
       <c r="F153" s="15"/>
       <c r="G153" s="15"/>
     </row>
-    <row r="154" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C154" s="15"/>
       <c r="D154" s="15"/>
       <c r="E154" s="15"/>
       <c r="F154" s="15"/>
       <c r="G154" s="15"/>
     </row>
-    <row r="155" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C155" s="15"/>
       <c r="D155" s="15"/>
       <c r="E155" s="15"/>
       <c r="F155" s="15"/>
       <c r="G155" s="15"/>
     </row>
-    <row r="156" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C156" s="15"/>
       <c r="D156" s="15"/>
       <c r="E156" s="15"/>
       <c r="F156" s="15"/>
       <c r="G156" s="15"/>
     </row>
-    <row r="157" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C157" s="15"/>
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
       <c r="F157" s="15"/>
       <c r="G157" s="15"/>
     </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C158" s="15"/>
       <c r="D158" s="15"/>
       <c r="E158" s="15"/>
       <c r="F158" s="15"/>
       <c r="G158" s="15"/>
     </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C159" s="15"/>
       <c r="D159" s="15"/>
       <c r="E159" s="15"/>
       <c r="F159" s="15"/>
       <c r="G159" s="15"/>
     </row>
-    <row r="160" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C160" s="15"/>
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
       <c r="F160" s="15"/>
       <c r="G160" s="15"/>
     </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C161" s="15"/>
       <c r="D161" s="15"/>
       <c r="E161" s="15"/>
       <c r="F161" s="15"/>
       <c r="G161" s="15"/>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C162" s="15"/>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
       <c r="F162" s="15"/>
       <c r="G162" s="15"/>
     </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C163" s="15"/>
       <c r="D163" s="15"/>
       <c r="E163" s="15"/>
       <c r="F163" s="15"/>
       <c r="G163" s="15"/>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C164" s="15"/>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
       <c r="F164" s="15"/>
       <c r="G164" s="15"/>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C165" s="15"/>
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
       <c r="F165" s="15"/>
       <c r="G165" s="15"/>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C166" s="15"/>
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
       <c r="F166" s="15"/>
       <c r="G166" s="15"/>
     </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C167" s="15"/>
       <c r="D167" s="15"/>
       <c r="E167" s="15"/>
       <c r="F167" s="15"/>
       <c r="G167" s="15"/>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C168" s="15"/>
       <c r="D168" s="15"/>
       <c r="E168" s="15"/>
       <c r="F168" s="15"/>
       <c r="G168" s="15"/>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C169" s="15"/>
       <c r="D169" s="15"/>
       <c r="E169" s="15"/>
       <c r="F169" s="15"/>
       <c r="G169" s="15"/>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C170" s="15"/>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
       <c r="F170" s="15"/>
       <c r="G170" s="15"/>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
       <c r="E171" s="15"/>
       <c r="F171" s="15"/>
       <c r="G171" s="15"/>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C172" s="15"/>
       <c r="D172" s="15"/>
       <c r="E172" s="15"/>
       <c r="F172" s="15"/>
       <c r="G172" s="15"/>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C173" s="15"/>
       <c r="D173" s="15"/>
       <c r="E173" s="15"/>
       <c r="F173" s="15"/>
       <c r="G173" s="15"/>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C174" s="15"/>
       <c r="D174" s="15"/>
       <c r="E174" s="15"/>
       <c r="F174" s="15"/>
       <c r="G174" s="15"/>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C175" s="15"/>
       <c r="D175" s="15"/>
       <c r="E175" s="15"/>
       <c r="F175" s="15"/>
       <c r="G175" s="15"/>
     </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C176" s="15"/>
       <c r="D176" s="15"/>
       <c r="E176" s="15"/>
       <c r="F176" s="15"/>
       <c r="G176" s="15"/>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C177" s="15"/>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
       <c r="F177" s="15"/>
       <c r="G177" s="15"/>
     </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="178" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C178" s="15"/>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
       <c r="F178" s="15"/>
       <c r="G178" s="15"/>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C179" s="15"/>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
       <c r="F179" s="15"/>
       <c r="G179" s="15"/>
     </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="180" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C180" s="15"/>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
       <c r="F180" s="15"/>
       <c r="G180" s="15"/>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="181" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C181" s="15"/>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
       <c r="F181" s="15"/>
       <c r="G181" s="15"/>
     </row>
-    <row r="182" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="182" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C182" s="15"/>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
       <c r="F182" s="15"/>
       <c r="G182" s="15"/>
     </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C183" s="15"/>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
       <c r="F183" s="15"/>
       <c r="G183" s="15"/>
     </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="184" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C184" s="15"/>
       <c r="D184" s="15"/>
       <c r="E184" s="15"/>
       <c r="F184" s="15"/>
       <c r="G184" s="15"/>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C185" s="15"/>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
       <c r="F185" s="15"/>
       <c r="G185" s="15"/>
     </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C186" s="15"/>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
       <c r="F186" s="15"/>
       <c r="G186" s="15"/>
     </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C187" s="15"/>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
       <c r="F187" s="15"/>
       <c r="G187" s="15"/>
     </row>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="188" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C188" s="15"/>
       <c r="D188" s="15"/>
       <c r="E188" s="15"/>
       <c r="F188" s="15"/>
       <c r="G188" s="15"/>
     </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C189" s="15"/>
       <c r="D189" s="15"/>
       <c r="E189" s="15"/>
       <c r="F189" s="15"/>
       <c r="G189" s="15"/>
     </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C190" s="15"/>
       <c r="D190" s="15"/>
       <c r="E190" s="15"/>
       <c r="F190" s="15"/>
       <c r="G190" s="15"/>
     </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="191" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="15"/>
       <c r="G191" s="15"/>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C192" s="15"/>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="15"/>
       <c r="G192" s="15"/>
     </row>
-    <row r="193" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="15"/>
       <c r="G193" s="15"/>
     </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C194" s="15"/>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="15"/>
       <c r="G194" s="15"/>
     </row>
-    <row r="195" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="195" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C195" s="15"/>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="15"/>
       <c r="G195" s="15"/>
     </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C196" s="15"/>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
       <c r="F196" s="15"/>
       <c r="G196" s="15"/>
     </row>
-    <row r="197" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="197" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="F197" s="15"/>
       <c r="G197" s="15"/>
     </row>
-    <row r="198" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C198" s="15"/>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="15"/>
       <c r="G198" s="15"/>
     </row>
-    <row r="199" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C199" s="15"/>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
       <c r="F199" s="15"/>
       <c r="G199" s="15"/>
     </row>
-    <row r="200" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C200" s="15"/>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
       <c r="F200" s="15"/>
       <c r="G200" s="15"/>
     </row>
-    <row r="201" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C201" s="15"/>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
       <c r="F201" s="15"/>
       <c r="G201" s="15"/>
     </row>
-    <row r="202" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C202" s="15"/>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
       <c r="F202" s="15"/>
       <c r="G202" s="15"/>
     </row>
-    <row r="203" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C203" s="15"/>
       <c r="D203" s="15"/>
       <c r="E203" s="15"/>
       <c r="F203" s="15"/>
       <c r="G203" s="15"/>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C204" s="15"/>
       <c r="D204" s="15"/>
       <c r="E204" s="15"/>
       <c r="F204" s="15"/>
       <c r="G204" s="15"/>
     </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C205" s="15"/>
       <c r="D205" s="15"/>
       <c r="E205" s="15"/>
       <c r="F205" s="15"/>
       <c r="G205" s="15"/>
     </row>
-    <row r="206" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="206" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C206" s="15"/>
       <c r="D206" s="15"/>
       <c r="E206" s="15"/>
       <c r="F206" s="15"/>
       <c r="G206" s="15"/>
     </row>
-    <row r="207" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C207" s="15"/>
       <c r="D207" s="15"/>
       <c r="E207" s="15"/>
       <c r="F207" s="15"/>
       <c r="G207" s="15"/>
     </row>
-    <row r="208" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="208" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C208" s="15"/>
       <c r="D208" s="15"/>
       <c r="E208" s="15"/>
       <c r="F208" s="15"/>
       <c r="G208" s="15"/>
     </row>
-    <row r="209" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C209" s="15"/>
       <c r="D209" s="15"/>
       <c r="E209" s="15"/>
       <c r="F209" s="15"/>
       <c r="G209" s="15"/>
     </row>
-    <row r="210" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C210" s="15"/>
       <c r="D210" s="15"/>
       <c r="E210" s="15"/>
       <c r="F210" s="15"/>
       <c r="G210" s="15"/>
     </row>
-    <row r="211" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C211" s="15"/>
       <c r="D211" s="15"/>
       <c r="E211" s="15"/>
       <c r="F211" s="15"/>
       <c r="G211" s="15"/>
     </row>
-    <row r="212" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C212" s="15"/>
       <c r="D212" s="15"/>
       <c r="E212" s="15"/>
       <c r="F212" s="15"/>
       <c r="G212" s="15"/>
     </row>
-    <row r="213" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C213" s="15"/>
       <c r="D213" s="15"/>
       <c r="E213" s="15"/>
       <c r="F213" s="15"/>
       <c r="G213" s="15"/>
     </row>
-    <row r="214" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C214" s="15"/>
       <c r="D214" s="15"/>
       <c r="E214" s="15"/>
       <c r="F214" s="15"/>
       <c r="G214" s="15"/>
     </row>
-    <row r="215" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C215" s="15"/>
       <c r="D215" s="15"/>
       <c r="E215" s="15"/>
       <c r="F215" s="15"/>
       <c r="G215" s="15"/>
     </row>
-    <row r="216" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="216" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C216" s="15"/>
       <c r="D216" s="15"/>
       <c r="E216" s="15"/>
       <c r="F216" s="15"/>
       <c r="G216" s="15"/>
     </row>
-    <row r="217" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C217" s="15"/>
       <c r="D217" s="15"/>
       <c r="E217" s="15"/>
       <c r="F217" s="15"/>
       <c r="G217" s="15"/>
     </row>
-    <row r="218" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C218" s="15"/>
       <c r="D218" s="15"/>
       <c r="E218" s="15"/>
       <c r="F218" s="15"/>
       <c r="G218" s="15"/>
     </row>
-    <row r="219" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C219" s="15"/>
       <c r="D219" s="15"/>
       <c r="E219" s="15"/>
       <c r="F219" s="15"/>
       <c r="G219" s="15"/>
     </row>
-    <row r="220" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C220" s="15"/>
       <c r="D220" s="15"/>
       <c r="E220" s="15"/>
       <c r="F220" s="15"/>
       <c r="G220" s="15"/>
     </row>
-    <row r="221" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C221" s="15"/>
       <c r="D221" s="15"/>
       <c r="E221" s="15"/>
       <c r="F221" s="15"/>
       <c r="G221" s="15"/>
     </row>
-    <row r="222" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C222" s="15"/>
       <c r="D222" s="15"/>
       <c r="E222" s="15"/>
       <c r="F222" s="15"/>
       <c r="G222" s="15"/>
     </row>
-    <row r="223" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C223" s="15"/>
       <c r="D223" s="15"/>
       <c r="E223" s="15"/>
       <c r="F223" s="15"/>
       <c r="G223" s="15"/>
     </row>
-    <row r="224" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C224" s="15"/>
       <c r="D224" s="15"/>
       <c r="E224" s="15"/>
       <c r="F224" s="15"/>
       <c r="G224" s="15"/>
     </row>
-    <row r="225" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C225" s="15"/>
       <c r="D225" s="15"/>
       <c r="E225" s="15"/>
       <c r="F225" s="15"/>
       <c r="G225" s="15"/>
     </row>
-    <row r="226" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C226" s="15"/>
       <c r="D226" s="15"/>
       <c r="E226" s="15"/>
       <c r="F226" s="15"/>
       <c r="G226" s="15"/>
     </row>
-    <row r="227" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C227" s="15"/>
       <c r="D227" s="15"/>
       <c r="E227" s="15"/>
       <c r="F227" s="15"/>
       <c r="G227" s="15"/>
     </row>
-    <row r="228" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C228" s="15"/>
       <c r="D228" s="15"/>
       <c r="E228" s="15"/>
       <c r="F228" s="15"/>
       <c r="G228" s="15"/>
     </row>
-    <row r="229" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C229" s="15"/>
       <c r="D229" s="15"/>
       <c r="E229" s="15"/>
       <c r="F229" s="15"/>
       <c r="G229" s="15"/>
     </row>
-    <row r="230" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C230" s="15"/>
       <c r="D230" s="15"/>
       <c r="E230" s="15"/>
       <c r="F230" s="15"/>
       <c r="G230" s="15"/>
     </row>
-    <row r="231" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C231" s="15"/>
       <c r="D231" s="15"/>
       <c r="E231" s="15"/>
       <c r="F231" s="15"/>
       <c r="G231" s="15"/>
     </row>
-    <row r="232" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C232" s="15"/>
       <c r="D232" s="15"/>
       <c r="E232" s="15"/>
       <c r="F232" s="15"/>
       <c r="G232" s="15"/>
     </row>
-    <row r="233" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C233" s="15"/>
       <c r="D233" s="15"/>
       <c r="E233" s="15"/>
       <c r="F233" s="15"/>
       <c r="G233" s="15"/>
     </row>
-    <row r="234" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C234" s="15"/>
       <c r="D234" s="15"/>
       <c r="E234" s="15"/>
       <c r="F234" s="15"/>
       <c r="G234" s="15"/>
     </row>
-    <row r="235" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C235" s="15"/>
       <c r="D235" s="15"/>
       <c r="E235" s="15"/>
       <c r="F235" s="15"/>
       <c r="G235" s="15"/>
     </row>
-    <row r="236" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C236" s="15"/>
       <c r="D236" s="15"/>
       <c r="E236" s="15"/>
       <c r="F236" s="15"/>
       <c r="G236" s="15"/>
     </row>
-    <row r="237" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C237" s="15"/>
       <c r="D237" s="15"/>
       <c r="E237" s="15"/>
       <c r="F237" s="15"/>
       <c r="G237" s="15"/>
     </row>
-    <row r="238" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C238" s="15"/>
       <c r="D238" s="15"/>
       <c r="E238" s="15"/>
       <c r="F238" s="15"/>
       <c r="G238" s="15"/>
     </row>
-    <row r="239" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C239" s="15"/>
       <c r="D239" s="15"/>
       <c r="E239" s="15"/>
       <c r="F239" s="15"/>
       <c r="G239" s="15"/>
     </row>
-    <row r="240" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C240" s="15"/>
       <c r="D240" s="15"/>
       <c r="E240" s="15"/>
       <c r="F240" s="15"/>
       <c r="G240" s="15"/>
     </row>
-    <row r="241" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C241" s="15"/>
       <c r="D241" s="15"/>
       <c r="E241" s="15"/>
       <c r="F241" s="15"/>
       <c r="G241" s="15"/>
     </row>
-    <row r="242" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C242" s="15"/>
       <c r="D242" s="15"/>
       <c r="E242" s="15"/>
       <c r="F242" s="15"/>
       <c r="G242" s="15"/>
     </row>
-    <row r="243" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C243" s="15"/>
       <c r="D243" s="15"/>
       <c r="E243" s="15"/>
       <c r="F243" s="15"/>
       <c r="G243" s="15"/>
     </row>
-    <row r="244" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C244" s="15"/>
       <c r="D244" s="15"/>
       <c r="E244" s="15"/>
       <c r="F244" s="15"/>
       <c r="G244" s="15"/>
     </row>
-    <row r="245" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C245" s="15"/>
       <c r="D245" s="15"/>
       <c r="E245" s="15"/>
       <c r="F245" s="15"/>
       <c r="G245" s="15"/>
     </row>
-    <row r="246" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C246" s="15"/>
       <c r="D246" s="15"/>
       <c r="E246" s="15"/>
       <c r="F246" s="15"/>
       <c r="G246" s="15"/>
     </row>
-    <row r="247" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C247" s="15"/>
       <c r="D247" s="15"/>
       <c r="E247" s="15"/>
       <c r="F247" s="15"/>
       <c r="G247" s="15"/>
     </row>
-    <row r="248" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C248" s="15"/>
       <c r="D248" s="15"/>
       <c r="E248" s="15"/>
       <c r="F248" s="15"/>
       <c r="G248" s="15"/>
     </row>
-    <row r="249" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C249" s="15"/>
       <c r="D249" s="15"/>
       <c r="E249" s="15"/>
       <c r="F249" s="15"/>
       <c r="G249" s="15"/>
     </row>
-    <row r="250" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C250" s="15"/>
       <c r="D250" s="15"/>
       <c r="E250" s="15"/>
       <c r="F250" s="15"/>
       <c r="G250" s="15"/>
     </row>
-    <row r="251" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C251" s="15"/>
       <c r="D251" s="15"/>
       <c r="E251" s="15"/>
       <c r="F251" s="15"/>
       <c r="G251" s="15"/>
     </row>
-    <row r="252" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C252" s="15"/>
       <c r="D252" s="15"/>
       <c r="E252" s="15"/>
       <c r="F252" s="15"/>
       <c r="G252" s="15"/>
     </row>
-    <row r="253" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C253" s="15"/>
       <c r="D253" s="15"/>
       <c r="E253" s="15"/>
       <c r="F253" s="15"/>
       <c r="G253" s="15"/>
     </row>
-    <row r="254" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C254" s="15"/>
       <c r="D254" s="15"/>
       <c r="E254" s="15"/>
       <c r="F254" s="15"/>
       <c r="G254" s="15"/>
     </row>
-    <row r="255" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="255" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C255" s="15"/>
       <c r="D255" s="15"/>
       <c r="E255" s="15"/>
       <c r="F255" s="15"/>
       <c r="G255" s="15"/>
     </row>
-    <row r="256" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C256" s="15"/>
       <c r="D256" s="15"/>
       <c r="E256" s="15"/>
       <c r="F256" s="15"/>
       <c r="G256" s="15"/>
     </row>
-    <row r="257" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="257" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C257" s="15"/>
       <c r="D257" s="15"/>
       <c r="E257" s="15"/>
       <c r="F257" s="15"/>
       <c r="G257" s="15"/>
     </row>
-    <row r="258" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="258" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C258" s="15"/>
       <c r="D258" s="15"/>
       <c r="E258" s="15"/>
       <c r="F258" s="15"/>
       <c r="G258" s="15"/>
     </row>
-    <row r="259" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="259" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C259" s="15"/>
       <c r="D259" s="15"/>
       <c r="E259" s="15"/>
       <c r="F259" s="15"/>
       <c r="G259" s="15"/>
     </row>
-    <row r="260" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="260" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C260" s="15"/>
       <c r="D260" s="15"/>
       <c r="E260" s="15"/>
       <c r="F260" s="15"/>
       <c r="G260" s="15"/>
     </row>
-    <row r="261" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="261" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C261" s="15"/>
       <c r="D261" s="15"/>
       <c r="E261" s="15"/>
       <c r="F261" s="15"/>
       <c r="G261" s="15"/>
     </row>
-    <row r="262" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="262" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C262" s="15"/>
       <c r="D262" s="15"/>
       <c r="E262" s="15"/>
       <c r="F262" s="15"/>
       <c r="G262" s="15"/>
     </row>
-    <row r="263" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="263" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C263" s="15"/>
       <c r="D263" s="15"/>
       <c r="E263" s="15"/>
       <c r="F263" s="15"/>
       <c r="G263" s="15"/>
     </row>
-    <row r="264" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="264" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C264" s="15"/>
       <c r="D264" s="15"/>
       <c r="E264" s="15"/>
       <c r="F264" s="15"/>
       <c r="G264" s="15"/>
     </row>
-    <row r="265" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="265" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C265" s="15"/>
       <c r="D265" s="15"/>
       <c r="E265" s="15"/>
       <c r="F265" s="15"/>
       <c r="G265" s="15"/>
     </row>
-    <row r="266" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="266" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C266" s="15"/>
       <c r="D266" s="15"/>
       <c r="E266" s="15"/>
       <c r="F266" s="15"/>
       <c r="G266" s="15"/>
     </row>
-    <row r="267" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="267" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C267" s="15"/>
       <c r="D267" s="15"/>
       <c r="E267" s="15"/>
       <c r="F267" s="15"/>
       <c r="G267" s="15"/>
     </row>
-    <row r="268" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="268" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C268" s="15"/>
       <c r="D268" s="15"/>
       <c r="E268" s="15"/>
       <c r="F268" s="15"/>
       <c r="G268" s="15"/>
     </row>
-    <row r="269" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="269" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C269" s="15"/>
       <c r="D269" s="15"/>
       <c r="E269" s="15"/>
       <c r="F269" s="15"/>
       <c r="G269" s="15"/>
     </row>
-    <row r="270" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="270" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C270" s="15"/>
       <c r="D270" s="15"/>
       <c r="E270" s="15"/>
       <c r="F270" s="15"/>
       <c r="G270" s="15"/>
     </row>
-    <row r="271" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="271" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C271" s="15"/>
       <c r="D271" s="15"/>
       <c r="E271" s="15"/>
       <c r="F271" s="15"/>
       <c r="G271" s="15"/>
     </row>
-    <row r="272" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="272" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C272" s="15"/>
       <c r="D272" s="15"/>
       <c r="E272" s="15"/>
       <c r="F272" s="15"/>
       <c r="G272" s="15"/>
     </row>
-    <row r="273" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="273" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C273" s="15"/>
       <c r="D273" s="15"/>
       <c r="E273" s="15"/>
       <c r="F273" s="15"/>
       <c r="G273" s="15"/>
     </row>
-    <row r="274" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="274" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C274" s="15"/>
       <c r="D274" s="15"/>
       <c r="E274" s="15"/>
       <c r="F274" s="15"/>
       <c r="G274" s="15"/>
     </row>
-    <row r="275" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="275" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C275" s="15"/>
       <c r="D275" s="15"/>
       <c r="E275" s="15"/>
       <c r="F275" s="15"/>
       <c r="G275" s="15"/>
     </row>
-    <row r="276" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="276" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C276" s="15"/>
       <c r="D276" s="15"/>
       <c r="E276" s="15"/>
       <c r="F276" s="15"/>
       <c r="G276" s="15"/>
     </row>
-    <row r="277" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="277" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C277" s="15"/>
       <c r="D277" s="15"/>
       <c r="E277" s="15"/>
       <c r="F277" s="15"/>
       <c r="G277" s="15"/>
     </row>
-    <row r="278" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="278" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C278" s="15"/>
       <c r="D278" s="15"/>
       <c r="E278" s="15"/>
       <c r="F278" s="15"/>
       <c r="G278" s="15"/>
     </row>
-    <row r="279" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="279" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C279" s="15"/>
       <c r="D279" s="15"/>
       <c r="E279" s="15"/>
       <c r="F279" s="15"/>
       <c r="G279" s="15"/>
     </row>
-    <row r="280" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="280" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C280" s="15"/>
       <c r="D280" s="15"/>
       <c r="E280" s="15"/>
       <c r="F280" s="15"/>
       <c r="G280" s="15"/>
     </row>
-    <row r="281" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C281" s="15"/>
       <c r="D281" s="15"/>
       <c r="E281" s="15"/>
       <c r="F281" s="15"/>
       <c r="G281" s="15"/>
     </row>
-    <row r="282" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C282" s="15"/>
       <c r="D282" s="15"/>
       <c r="E282" s="15"/>
       <c r="F282" s="15"/>
       <c r="G282" s="15"/>
     </row>
-    <row r="283" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="283" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C283" s="15"/>
       <c r="D283" s="15"/>
       <c r="E283" s="15"/>
       <c r="F283" s="15"/>
       <c r="G283" s="15"/>
     </row>
-    <row r="284" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="284" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C284" s="15"/>
       <c r="D284" s="15"/>
       <c r="E284" s="15"/>
       <c r="F284" s="15"/>
       <c r="G284" s="15"/>
     </row>
-    <row r="285" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="285" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C285" s="15"/>
       <c r="D285" s="15"/>
       <c r="E285" s="15"/>
       <c r="F285" s="15"/>
       <c r="G285" s="15"/>
     </row>
-    <row r="286" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="286" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C286" s="15"/>
       <c r="D286" s="15"/>
       <c r="E286" s="15"/>
       <c r="F286" s="15"/>
       <c r="G286" s="15"/>
     </row>
-    <row r="287" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C287" s="15"/>
       <c r="D287" s="15"/>
       <c r="E287" s="15"/>
       <c r="F287" s="15"/>
       <c r="G287" s="15"/>
     </row>
-    <row r="288" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="288" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C288" s="15"/>
       <c r="D288" s="15"/>
       <c r="E288" s="15"/>
       <c r="F288" s="15"/>
       <c r="G288" s="15"/>
     </row>
-    <row r="289" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="289" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C289" s="15"/>
       <c r="D289" s="15"/>
       <c r="E289" s="15"/>
       <c r="F289" s="15"/>
       <c r="G289" s="15"/>
     </row>
-    <row r="290" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="290" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C290" s="15"/>
       <c r="D290" s="15"/>
       <c r="E290" s="15"/>
       <c r="F290" s="15"/>
       <c r="G290" s="15"/>
     </row>
-    <row r="291" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="291" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C291" s="15"/>
       <c r="D291" s="15"/>
       <c r="E291" s="15"/>
       <c r="F291" s="15"/>
       <c r="G291" s="15"/>
     </row>
-    <row r="292" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="292" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C292" s="15"/>
       <c r="D292" s="15"/>
       <c r="E292" s="15"/>
       <c r="F292" s="15"/>
       <c r="G292" s="15"/>
     </row>
-    <row r="293" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="293" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C293" s="15"/>
       <c r="D293" s="15"/>
       <c r="E293" s="15"/>
       <c r="F293" s="15"/>
       <c r="G293" s="15"/>
     </row>
-    <row r="294" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="294" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C294" s="15"/>
       <c r="D294" s="15"/>
       <c r="E294" s="15"/>
       <c r="F294" s="15"/>
       <c r="G294" s="15"/>
     </row>
-    <row r="295" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="295" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C295" s="15"/>
       <c r="D295" s="15"/>
       <c r="E295" s="15"/>
       <c r="F295" s="15"/>
       <c r="G295" s="15"/>
     </row>
-    <row r="296" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="296" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C296" s="15"/>
       <c r="D296" s="15"/>
       <c r="E296" s="15"/>
       <c r="F296" s="15"/>
       <c r="G296" s="15"/>
     </row>
-    <row r="297" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="297" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C297" s="15"/>
       <c r="D297" s="15"/>
       <c r="E297" s="15"/>
       <c r="F297" s="15"/>
       <c r="G297" s="15"/>
     </row>
-    <row r="298" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="298" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C298" s="15"/>
       <c r="D298" s="15"/>
       <c r="E298" s="15"/>
       <c r="F298" s="15"/>
       <c r="G298" s="15"/>
     </row>
-    <row r="299" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="299" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C299" s="15"/>
       <c r="D299" s="15"/>
       <c r="E299" s="15"/>
       <c r="F299" s="15"/>
       <c r="G299" s="15"/>
     </row>
-    <row r="300" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="300" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C300" s="15"/>
       <c r="D300" s="15"/>
       <c r="E300" s="15"/>
       <c r="F300" s="15"/>
       <c r="G300" s="15"/>
     </row>
-    <row r="301" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="301" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C301" s="15"/>
       <c r="D301" s="15"/>
       <c r="E301" s="15"/>
       <c r="F301" s="15"/>
       <c r="G301" s="15"/>
     </row>
-    <row r="302" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="302" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C302" s="15"/>
       <c r="D302" s="15"/>
       <c r="E302" s="15"/>
       <c r="F302" s="15"/>
       <c r="G302" s="15"/>
     </row>
-    <row r="303" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="303" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C303" s="15"/>
       <c r="D303" s="15"/>
       <c r="E303" s="15"/>
       <c r="F303" s="15"/>
       <c r="G303" s="15"/>
     </row>
-    <row r="304" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="304" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C304" s="15"/>
       <c r="D304" s="15"/>
       <c r="E304" s="15"/>
       <c r="F304" s="15"/>
       <c r="G304" s="15"/>
     </row>
-    <row r="305" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C305" s="15"/>
       <c r="D305" s="15"/>
       <c r="E305" s="15"/>
       <c r="F305" s="15"/>
       <c r="G305" s="15"/>
     </row>
-    <row r="306" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C306" s="15"/>
       <c r="D306" s="15"/>
       <c r="E306" s="15"/>
       <c r="F306" s="15"/>
       <c r="G306" s="15"/>
     </row>
-    <row r="307" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C307" s="15"/>
       <c r="D307" s="15"/>
       <c r="E307" s="15"/>
       <c r="F307" s="15"/>
       <c r="G307" s="15"/>
     </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C308" s="15"/>
       <c r="D308" s="15"/>
       <c r="E308" s="15"/>
       <c r="F308" s="15"/>
       <c r="G308" s="15"/>
     </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C309" s="15"/>
       <c r="D309" s="15"/>
       <c r="E309" s="15"/>
       <c r="F309" s="15"/>
       <c r="G309" s="15"/>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C310" s="15"/>
       <c r="D310" s="15"/>
       <c r="E310" s="15"/>
       <c r="F310" s="15"/>
       <c r="G310" s="15"/>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C311" s="15"/>
       <c r="D311" s="15"/>
       <c r="E311" s="15"/>
       <c r="F311" s="15"/>
       <c r="G311" s="15"/>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C312" s="15"/>
       <c r="D312" s="15"/>
       <c r="E312" s="15"/>
       <c r="F312" s="15"/>
       <c r="G312" s="15"/>
     </row>
-    <row r="313" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C313" s="15"/>
       <c r="D313" s="15"/>
       <c r="E313" s="15"/>
       <c r="F313" s="15"/>
       <c r="G313" s="15"/>
     </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C314" s="15"/>
       <c r="D314" s="15"/>
       <c r="E314" s="15"/>
       <c r="F314" s="15"/>
       <c r="G314" s="15"/>
     </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C315" s="15"/>
       <c r="D315" s="15"/>
       <c r="E315" s="15"/>
       <c r="F315" s="15"/>
       <c r="G315" s="15"/>
     </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C316" s="15"/>
       <c r="D316" s="15"/>
       <c r="E316" s="15"/>
       <c r="F316" s="15"/>
       <c r="G316" s="15"/>
     </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C317" s="15"/>
       <c r="D317" s="15"/>
       <c r="E317" s="15"/>
       <c r="F317" s="15"/>
       <c r="G317" s="15"/>
     </row>
-    <row r="318" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C318" s="15"/>
       <c r="D318" s="15"/>
       <c r="E318" s="15"/>
       <c r="F318" s="15"/>
       <c r="G318" s="15"/>
     </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C319" s="15"/>
       <c r="D319" s="15"/>
       <c r="E319" s="15"/>
       <c r="F319" s="15"/>
       <c r="G319" s="15"/>
     </row>
-    <row r="320" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="320" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C320" s="15"/>
       <c r="D320" s="15"/>
       <c r="E320" s="15"/>
       <c r="F320" s="15"/>
       <c r="G320" s="15"/>
     </row>
-    <row r="321" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="321" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C321" s="15"/>
       <c r="D321" s="15"/>
       <c r="E321" s="15"/>
       <c r="F321" s="15"/>
       <c r="G321" s="15"/>
     </row>
-    <row r="322" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="322" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C322" s="15"/>
       <c r="D322" s="15"/>
       <c r="E322" s="15"/>
       <c r="F322" s="15"/>
       <c r="G322" s="15"/>
     </row>
-    <row r="323" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="323" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C323" s="15"/>
       <c r="D323" s="15"/>
       <c r="E323" s="15"/>
       <c r="F323" s="15"/>
       <c r="G323" s="15"/>
     </row>
-    <row r="324" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="324" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C324" s="15"/>
       <c r="D324" s="15"/>
       <c r="E324" s="15"/>
       <c r="F324" s="15"/>
       <c r="G324" s="15"/>
     </row>
-    <row r="325" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="325" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C325" s="15"/>
       <c r="D325" s="15"/>
       <c r="E325" s="15"/>
       <c r="F325" s="15"/>
       <c r="G325" s="15"/>
     </row>
-    <row r="326" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="326" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C326" s="15"/>
       <c r="D326" s="15"/>
       <c r="E326" s="15"/>
       <c r="F326" s="15"/>
       <c r="G326" s="15"/>
     </row>
-    <row r="327" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="327" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C327" s="15"/>
       <c r="D327" s="15"/>
       <c r="E327" s="15"/>
       <c r="F327" s="15"/>
       <c r="G327" s="15"/>
     </row>
-    <row r="328" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="328" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C328" s="15"/>
       <c r="D328" s="15"/>
       <c r="E328" s="15"/>
       <c r="F328" s="15"/>
       <c r="G328" s="15"/>
     </row>
-    <row r="329" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="329" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C329" s="15"/>
       <c r="D329" s="15"/>
       <c r="E329" s="15"/>
       <c r="F329" s="15"/>
       <c r="G329" s="15"/>
     </row>
-    <row r="330" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="330" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C330" s="15"/>
       <c r="D330" s="15"/>
       <c r="E330" s="15"/>
       <c r="F330" s="15"/>
       <c r="G330" s="15"/>
     </row>
-    <row r="331" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="331" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C331" s="15"/>
       <c r="D331" s="15"/>
       <c r="E331" s="15"/>
       <c r="F331" s="15"/>
       <c r="G331" s="15"/>
     </row>
-    <row r="332" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="332" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C332" s="15"/>
       <c r="D332" s="15"/>
       <c r="E332" s="15"/>
       <c r="F332" s="15"/>
       <c r="G332" s="15"/>
     </row>
-    <row r="333" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="333" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C333" s="15"/>
       <c r="D333" s="15"/>
       <c r="E333" s="15"/>
       <c r="F333" s="15"/>
       <c r="G333" s="15"/>
     </row>
-    <row r="334" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="334" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C334" s="15"/>
       <c r="D334" s="15"/>
       <c r="E334" s="15"/>
       <c r="F334" s="15"/>
       <c r="G334" s="15"/>
     </row>
-    <row r="335" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="335" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C335" s="15"/>
       <c r="D335" s="15"/>
       <c r="E335" s="15"/>
       <c r="F335" s="15"/>
       <c r="G335" s="15"/>
     </row>
-    <row r="336" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="336" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C336" s="15"/>
       <c r="D336" s="15"/>
       <c r="E336" s="15"/>
       <c r="F336" s="15"/>
       <c r="G336" s="15"/>
     </row>
-    <row r="337" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="337" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C337" s="15"/>
       <c r="D337" s="15"/>
       <c r="E337" s="15"/>
       <c r="F337" s="15"/>
       <c r="G337" s="15"/>
     </row>
-    <row r="338" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="338" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C338" s="15"/>
       <c r="D338" s="15"/>
       <c r="E338" s="15"/>
       <c r="F338" s="15"/>
       <c r="G338" s="15"/>
     </row>
-    <row r="339" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="339" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C339" s="15"/>
       <c r="D339" s="15"/>
       <c r="E339" s="15"/>
       <c r="F339" s="15"/>
       <c r="G339" s="15"/>
     </row>
-    <row r="340" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C340" s="15"/>
       <c r="D340" s="15"/>
       <c r="E340" s="15"/>
       <c r="F340" s="15"/>
       <c r="G340" s="15"/>
     </row>
-    <row r="341" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C341" s="15"/>
       <c r="D341" s="15"/>
       <c r="E341" s="15"/>
       <c r="F341" s="15"/>
       <c r="G341" s="15"/>
     </row>
-    <row r="342" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="342" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C342" s="15"/>
       <c r="D342" s="15"/>
       <c r="E342" s="15"/>
       <c r="F342" s="15"/>
       <c r="G342" s="15"/>
     </row>
-    <row r="343" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="343" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C343" s="15"/>
       <c r="D343" s="15"/>
       <c r="E343" s="15"/>
       <c r="F343" s="15"/>
       <c r="G343" s="15"/>
     </row>
-    <row r="344" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="344" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C344" s="15"/>
       <c r="D344" s="15"/>
       <c r="E344" s="15"/>
       <c r="F344" s="15"/>
       <c r="G344" s="15"/>
     </row>
-    <row r="345" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="345" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C345" s="15"/>
       <c r="D345" s="15"/>
       <c r="E345" s="15"/>
       <c r="F345" s="15"/>
       <c r="G345" s="15"/>
     </row>
-    <row r="346" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="346" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C346" s="15"/>
       <c r="D346" s="15"/>
       <c r="E346" s="15"/>
       <c r="F346" s="15"/>
       <c r="G346" s="15"/>
     </row>
-    <row r="347" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C347" s="15"/>
       <c r="D347" s="15"/>
       <c r="E347" s="15"/>
       <c r="F347" s="15"/>
       <c r="G347" s="15"/>
     </row>
-    <row r="348" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C348" s="15"/>
       <c r="D348" s="15"/>
       <c r="E348" s="15"/>
       <c r="F348" s="15"/>
       <c r="G348" s="15"/>
     </row>
-    <row r="349" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C349" s="15"/>
       <c r="D349" s="15"/>
       <c r="E349" s="15"/>
       <c r="F349" s="15"/>
       <c r="G349" s="15"/>
     </row>
-    <row r="350" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="350" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C350" s="15"/>
       <c r="D350" s="15"/>
       <c r="E350" s="15"/>
       <c r="F350" s="15"/>
       <c r="G350" s="15"/>
     </row>
-    <row r="351" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="351" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C351" s="15"/>
       <c r="D351" s="15"/>
       <c r="E351" s="15"/>
       <c r="F351" s="15"/>
       <c r="G351" s="15"/>
     </row>
-    <row r="352" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="352" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C352" s="15"/>
       <c r="D352" s="15"/>
       <c r="E352" s="15"/>
       <c r="F352" s="15"/>
       <c r="G352" s="15"/>
     </row>
-    <row r="353" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="353" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C353" s="15"/>
       <c r="D353" s="15"/>
       <c r="E353" s="15"/>
       <c r="F353" s="15"/>
       <c r="G353" s="15"/>
     </row>
-    <row r="354" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="354" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C354" s="15"/>
       <c r="D354" s="15"/>
       <c r="E354" s="15"/>
       <c r="F354" s="15"/>
       <c r="G354" s="15"/>
     </row>
-    <row r="355" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C355" s="15"/>
       <c r="D355" s="15"/>
       <c r="E355" s="15"/>
       <c r="F355" s="15"/>
       <c r="G355" s="15"/>
     </row>
-    <row r="356" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="356" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C356" s="15"/>
       <c r="D356" s="15"/>
       <c r="E356" s="15"/>
       <c r="F356" s="15"/>
       <c r="G356" s="15"/>
     </row>
-    <row r="357" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C357" s="15"/>
       <c r="D357" s="15"/>
       <c r="E357" s="15"/>
       <c r="F357" s="15"/>
       <c r="G357" s="15"/>
     </row>
-    <row r="358" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C358" s="15"/>
       <c r="D358" s="15"/>
       <c r="E358" s="15"/>
       <c r="F358" s="15"/>
       <c r="G358" s="15"/>
     </row>
-    <row r="359" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C359" s="15"/>
       <c r="D359" s="15"/>
       <c r="E359" s="15"/>
       <c r="F359" s="15"/>
       <c r="G359" s="15"/>
     </row>
-    <row r="360" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="360" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C360" s="15"/>
       <c r="D360" s="15"/>
       <c r="E360" s="15"/>
       <c r="F360" s="15"/>
       <c r="G360" s="15"/>
     </row>
-    <row r="361" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="361" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C361" s="15"/>
       <c r="D361" s="15"/>
       <c r="E361" s="15"/>
       <c r="F361" s="15"/>
       <c r="G361" s="15"/>
     </row>
-    <row r="362" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C362" s="15"/>
       <c r="D362" s="15"/>
       <c r="E362" s="15"/>
       <c r="F362" s="15"/>
       <c r="G362" s="15"/>
     </row>
-    <row r="363" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C363" s="15"/>
       <c r="D363" s="15"/>
       <c r="E363" s="15"/>
       <c r="F363" s="15"/>
       <c r="G363" s="15"/>
     </row>
-    <row r="364" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="364" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C364" s="15"/>
       <c r="D364" s="15"/>
       <c r="E364" s="15"/>
       <c r="F364" s="15"/>
       <c r="G364" s="15"/>
     </row>
-    <row r="365" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="365" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C365" s="15"/>
       <c r="D365" s="15"/>
       <c r="E365" s="15"/>
       <c r="F365" s="15"/>
       <c r="G365" s="15"/>
     </row>
-    <row r="366" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="366" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C366" s="15"/>
       <c r="D366" s="15"/>
       <c r="E366" s="15"/>
       <c r="F366" s="15"/>
       <c r="G366" s="15"/>
     </row>
-    <row r="367" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="367" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C367" s="15"/>
       <c r="D367" s="15"/>
       <c r="E367" s="15"/>
       <c r="F367" s="15"/>
       <c r="G367" s="15"/>
     </row>
-    <row r="368" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C368" s="15"/>
       <c r="D368" s="15"/>
       <c r="E368" s="15"/>
       <c r="F368" s="15"/>
       <c r="G368" s="15"/>
     </row>
-    <row r="369" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="369" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C369" s="15"/>
       <c r="D369" s="15"/>
       <c r="E369" s="15"/>
       <c r="F369" s="15"/>
       <c r="G369" s="15"/>
     </row>
-    <row r="370" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C370" s="15"/>
       <c r="D370" s="15"/>
       <c r="E370" s="15"/>
       <c r="F370" s="15"/>
       <c r="G370" s="15"/>
     </row>
-    <row r="371" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C371" s="15"/>
       <c r="D371" s="15"/>
       <c r="E371" s="15"/>
       <c r="F371" s="15"/>
       <c r="G371" s="15"/>
     </row>
-    <row r="372" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C372" s="15"/>
       <c r="D372" s="15"/>
       <c r="E372" s="15"/>
       <c r="F372" s="15"/>
       <c r="G372" s="15"/>
     </row>
-    <row r="373" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C373" s="15"/>
       <c r="D373" s="15"/>
       <c r="E373" s="15"/>
       <c r="F373" s="15"/>
       <c r="G373" s="15"/>
     </row>
-    <row r="374" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C374" s="15"/>
       <c r="D374" s="15"/>
       <c r="E374" s="15"/>
       <c r="F374" s="15"/>
       <c r="G374" s="15"/>
     </row>
-    <row r="375" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C375" s="15"/>
       <c r="D375" s="15"/>
       <c r="E375" s="15"/>
       <c r="F375" s="15"/>
       <c r="G375" s="15"/>
     </row>
-    <row r="376" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C376" s="15"/>
       <c r="D376" s="15"/>
       <c r="E376" s="15"/>
       <c r="F376" s="15"/>
       <c r="G376" s="15"/>
     </row>
-    <row r="377" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="377" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C377" s="15"/>
       <c r="D377" s="15"/>
       <c r="E377" s="15"/>
       <c r="F377" s="15"/>
       <c r="G377" s="15"/>
     </row>
-    <row r="378" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C378" s="15"/>
       <c r="D378" s="15"/>
       <c r="E378" s="15"/>
       <c r="F378" s="15"/>
       <c r="G378" s="15"/>
     </row>
-    <row r="379" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C379" s="15"/>
       <c r="D379" s="15"/>
       <c r="E379" s="15"/>
       <c r="F379" s="15"/>
       <c r="G379" s="15"/>
     </row>
-    <row r="380" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C380" s="15"/>
       <c r="D380" s="15"/>
       <c r="E380" s="15"/>
@@ -11878,7 +12088,10 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="A1:DG2"/>
     <mergeCell ref="C57:C59"/>
     <mergeCell ref="C60:C65"/>
     <mergeCell ref="C66:C68"/>
@@ -11888,9 +12101,6 @@
     <mergeCell ref="C30:C39"/>
     <mergeCell ref="C40:C47"/>
     <mergeCell ref="C48:C56"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:K68">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Not Ok">
@@ -11913,29 +12123,29 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B11" location="'TBP_80-512516'!Print_Titles" display="'TBP_80-512516'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B12" location="'TBP_80-512517'!Print_Titles" display="'TBP_80-512517'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B13" location="'TBP_80-512518'!Print_Titles" display="'TBP_80-512518'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B14" location="'TBP_80-512519'!Print_Titles" display="'TBP_80-512519'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B15" location="'TBP_80-512520'!Print_Titles" display="'TBP_80-512520'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B16" location="'TBP_80-512521'!Print_Titles" display="'TBP_80-512521'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B17" location="'TBP_80-512522'!Print_Titles" display="'TBP_80-512522'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B18" location="'TBP_80-512523'!Print_Titles" display="'TBP_80-512523'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B19" location="'TBP_50-512306'!Print_Titles" display="'TBP_50-512306'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B23" location="'TBP_50-512310'!Print_Titles" display="'TBP_50-512310'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B22" location="'TBP_50-512309'!Print_Titles" display="'TBP_50-512309'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B21" location="'TBP_50-512308'!Print_Titles" display="'TBP_50-512308'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B20" location="'TBP_50-512307'!Print_Titles" display="'TBP_50-512307'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B27" location="'H113-13'!Print_Titles" display="'H113-13'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B26" location="'H112-13'!Print_Titles" display="'H112-13'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B25" location="'H111-13'!Print_Titles" display="'H111-13'!Print_Titles" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B24" location="'H110-13'!Print_Titles" display="'H110-13'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B35" location="'NB_89'!Print_Titles" display="'NB_89'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B34" location="'NB_88'!Print_Titles" display="'NB_88'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B33" location="'NB_87'!Print_Titles" display="'NB_87'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B32" location="'NB_86'!Print_Titles" display="'NB_86'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B31" location="'NB_85'!Print_Titles" display="'NB_85'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B30" location="'NB_84_'!Print_Titles" display="'NB_84_'!Print_Titles" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B11" location="'TBP_80-512516'!Print_Titles" display="'TBP_80-512516'!Print_Titles"/>
+    <hyperlink ref="B12" location="'TBP_80-512517'!Print_Titles" display="'TBP_80-512517'!Print_Titles"/>
+    <hyperlink ref="B13" location="'TBP_80-512518'!Print_Titles" display="'TBP_80-512518'!Print_Titles"/>
+    <hyperlink ref="B14" location="'TBP_80-512519'!Print_Titles" display="'TBP_80-512519'!Print_Titles"/>
+    <hyperlink ref="B15" location="'TBP_80-512520'!Print_Titles" display="'TBP_80-512520'!Print_Titles"/>
+    <hyperlink ref="B16" location="'TBP_80-512521'!Print_Titles" display="'TBP_80-512521'!Print_Titles"/>
+    <hyperlink ref="B17" location="'TBP_80-512522'!Print_Titles" display="'TBP_80-512522'!Print_Titles"/>
+    <hyperlink ref="B18" location="'TBP_80-512523'!Print_Titles" display="'TBP_80-512523'!Print_Titles"/>
+    <hyperlink ref="B19" location="'TBP_50-512306'!Print_Titles" display="'TBP_50-512306'!Print_Titles"/>
+    <hyperlink ref="B23" location="'TBP_50-512310'!Print_Titles" display="'TBP_50-512310'!Print_Titles"/>
+    <hyperlink ref="B22" location="'TBP_50-512309'!Print_Titles" display="'TBP_50-512309'!Print_Titles"/>
+    <hyperlink ref="B21" location="'TBP_50-512308'!Print_Titles" display="'TBP_50-512308'!Print_Titles"/>
+    <hyperlink ref="B20" location="'TBP_50-512307'!Print_Titles" display="'TBP_50-512307'!Print_Titles"/>
+    <hyperlink ref="B27" location="'H113-13'!Print_Titles" display="'H113-13'!Print_Titles"/>
+    <hyperlink ref="B26" location="'H112-13'!Print_Titles" display="'H112-13'!Print_Titles"/>
+    <hyperlink ref="B25" location="'H111-13'!Print_Titles" display="'H111-13'!Print_Titles"/>
+    <hyperlink ref="B24" location="'H110-13'!Print_Titles" display="'H110-13'!Print_Titles"/>
+    <hyperlink ref="B35" location="'NB_89'!Print_Titles" display="'NB_89'!Print_Titles"/>
+    <hyperlink ref="B34" location="'NB_88'!Print_Titles" display="'NB_88'!Print_Titles"/>
+    <hyperlink ref="B33" location="'NB_87'!Print_Titles" display="'NB_87'!Print_Titles"/>
+    <hyperlink ref="B32" location="'NB_86'!Print_Titles" display="'NB_86'!Print_Titles"/>
+    <hyperlink ref="B31" location="'NB_85'!Print_Titles" display="'NB_85'!Print_Titles"/>
+    <hyperlink ref="B30" location="'NB_84_'!Print_Titles" display="'NB_84_'!Print_Titles"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>